<commit_message>
voigt profile fits + better notebook format
Made the spreadsheet plotter much prettier. Also ran fits in PyMca using the voigt profile instead of hypermet. (fits_out_I)
</commit_message>
<xml_diff>
--- a/GaP thickness series.xlsx
+++ b/GaP thickness series.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elf\Documents\GitHub\xrf-thickness-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92964BB0-A187-4405-B1D2-D62641882DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB59F61-C652-4D60-AFF4-343F304A0AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>sample number</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>BG included, d1</t>
+  </si>
+  <si>
+    <t>very inhomogenous</t>
   </si>
 </sst>
 </file>
@@ -267,6 +270,64 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>data!$B$3:$B$7</c:f>
@@ -901,6 +962,64 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>data!$B$3:$B$7</c:f>
@@ -4133,14 +4252,14 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4319,6 +4438,9 @@
       </c>
       <c r="B14">
         <v>450</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -4369,8 +4491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2848C461-DB02-413D-AC3C-422114C127E3}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
P plots in excel spreadsheet
</commit_message>
<xml_diff>
--- a/GaP thickness series.xlsx
+++ b/GaP thickness series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elf\Documents\GitHub\xrf-thickness-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB59F61-C652-4D60-AFF4-343F304A0AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB58CE5-D4CD-4F70-ACA9-5D8832DF9FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
   </bookViews>
   <sheets>
     <sheet name="GaP thickness series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>sample number</t>
   </si>
@@ -116,6 +116,20 @@
   </si>
   <si>
     <t>very inhomogenous</t>
+  </si>
+  <si>
+    <r>
+      <t>P K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>α intensity</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1046,7 +1060,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$F$3:$F$7</c:f>
+              <c:f>data!$G$3:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1363,7 +1377,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$G$3:$G$7</c:f>
+              <c:f>data!$H$3:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1579,6 +1593,351 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>290.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$F$3:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4854</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6061</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11507</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26453</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D35F-4BD8-9A6E-1162B2FF27D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="621838888"/>
+        <c:axId val="621835608"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="621838888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621835608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="621835608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621838888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1739,6 +2098,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3803,17 +4202,533 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
@@ -3843,13 +4758,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
@@ -3879,13 +4794,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
@@ -3915,13 +4830,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
@@ -3944,6 +4859,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{387DA0A1-1E89-3E3C-0475-032C360E7AAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4251,7 +5202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36829E-C274-49DF-95D4-E8318511F9CD}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -4489,10 +5440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2848C461-DB02-413D-AC3C-422114C127E3}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4502,17 +5453,18 @@
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -4529,13 +5481,16 @@
         <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3158</v>
       </c>
@@ -4552,13 +5507,16 @@
         <v>340076</v>
       </c>
       <c r="F3">
+        <v>4854</v>
+      </c>
+      <c r="G3">
         <v>15115</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>340359</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2802</v>
       </c>
@@ -4572,13 +5530,16 @@
         <v>325113</v>
       </c>
       <c r="F4">
+        <v>6061</v>
+      </c>
+      <c r="G4">
         <v>18495</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>325371</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2808</v>
       </c>
@@ -4592,13 +5553,16 @@
         <v>317502</v>
       </c>
       <c r="F5">
+        <v>7168</v>
+      </c>
+      <c r="G5">
         <v>21941</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>317822</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2555</v>
       </c>
@@ -4615,13 +5579,16 @@
         <v>290865</v>
       </c>
       <c r="F6">
+        <v>11507</v>
+      </c>
+      <c r="G6">
         <v>35605</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>291108</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2546</v>
       </c>
@@ -4638,16 +5605,19 @@
         <v>208416</v>
       </c>
       <c r="F7">
+        <v>26453</v>
+      </c>
+      <c r="G7">
         <v>91449</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>208659</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added 2566 data and plotter additions
imported data from cvd2566 and added new option to the plotter to make heatmap plot with imshow()
</commit_message>
<xml_diff>
--- a/GaP thickness series.xlsx
+++ b/GaP thickness series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elf\Documents\GitHub\xrf-thickness-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB58CE5-D4CD-4F70-ACA9-5D8832DF9FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08462288-2D1F-4DA5-8A0F-2244B7723D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
   </bookViews>
   <sheets>
     <sheet name="GaP thickness series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>sample number</t>
   </si>
@@ -5202,8 +5202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36829E-C274-49DF-95D4-E8318511F9CD}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5211,8 +5211,9 @@
     <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5396,9 +5397,7 @@
       <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -5442,7 +5441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2848C461-DB02-413D-AC3C-422114C127E3}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added second 2546 high res scan
</commit_message>
<xml_diff>
--- a/GaP thickness series.xlsx
+++ b/GaP thickness series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elf\Documents\GitHub\xrf-thickness-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757A1796-9D72-4CD5-AAAB-257AC47EA6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD31DFD4-3FAB-4AC7-A9EB-89A280E81765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
   </bookViews>
   <sheets>
     <sheet name="GaP thickness series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>sample number</t>
   </si>
@@ -157,18 +157,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -198,7 +192,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5209,8 +5202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36829E-C274-49DF-95D4-E8318511F9CD}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5256,7 +5249,9 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -5268,7 +5263,9 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -5301,7 +5298,9 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -5328,7 +5327,9 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -5367,7 +5368,9 @@
       <c r="E11" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -5379,7 +5382,9 @@
       <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -5427,7 +5432,9 @@
       <c r="E16" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -5443,10 +5450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2848C461-DB02-413D-AC3C-422114C127E3}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5526,6 +5533,9 @@
       <c r="B4">
         <v>51.5</v>
       </c>
+      <c r="C4">
+        <v>51.59</v>
+      </c>
       <c r="D4">
         <v>16549</v>
       </c>
@@ -5549,6 +5559,9 @@
       <c r="B5">
         <v>62.5</v>
       </c>
+      <c r="C5">
+        <v>62.31</v>
+      </c>
       <c r="D5">
         <v>19931</v>
       </c>
@@ -5599,7 +5612,7 @@
         <v>290.7</v>
       </c>
       <c r="C7">
-        <v>285.86</v>
+        <v>285.37</v>
       </c>
       <c r="D7">
         <v>89404</v>
@@ -5615,6 +5628,14 @@
       </c>
       <c r="H7">
         <v>208659</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3076</v>
+      </c>
+      <c r="C8">
+        <v>547.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split batch processor into pymca and bruker
main motivation for this is that pymca distinguishes between different lines for the same element, while bruker just tells you the total counts for a certain element
</commit_message>
<xml_diff>
--- a/GaP thickness series.xlsx
+++ b/GaP thickness series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elf\Documents\GitHub\xrf-thickness-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB234A95-7420-4544-8145-E4696586B4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C99688-3D5B-4B4B-8EA9-C0EA8A497B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{30E33E6E-91C0-4B0D-915F-08E95790EBAA}"/>
   </bookViews>
   <sheets>
     <sheet name="GaP thickness series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>sample number</t>
   </si>
@@ -109,12 +109,6 @@
     </r>
   </si>
   <si>
-    <t>no BG, d1</t>
-  </si>
-  <si>
-    <t>BG included, d1</t>
-  </si>
-  <si>
     <t>very inhomogenous</t>
   </si>
   <si>
@@ -130,6 +124,18 @@
       </rPr>
       <t>α intensity</t>
     </r>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Bruker, no BG, d1</t>
+  </si>
+  <si>
+    <t>Bruker, BG included, d1</t>
+  </si>
+  <si>
+    <t>P K</t>
   </si>
 </sst>
 </file>
@@ -1608,6 +1614,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>XRR thickness v P</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> intensity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1693,8 +1729,38 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1722,24 +1788,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$F$3:$F$7</c:f>
+              <c:f>data!$C$3:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4854</c:v>
+                  <c:v>41.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6061</c:v>
+                  <c:v>51.59</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7168</c:v>
+                  <c:v>62.31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11507</c:v>
+                  <c:v>106.59</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26453</c:v>
+                  <c:v>285.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1747,7 +1813,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D35F-4BD8-9A6E-1162B2FF27D6}"/>
+              <c16:uniqueId val="{00000000-E480-4932-8F73-71EA2995F019}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1759,11 +1825,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="621838888"/>
-        <c:axId val="621835608"/>
+        <c:axId val="432808664"/>
+        <c:axId val="432803416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="621838888"/>
+        <c:axId val="432808664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,12 +1886,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="621835608"/>
+        <c:crossAx val="432803416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="621835608"/>
+        <c:axId val="432803416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,7 +1948,413 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="621838888"/>
+        <c:crossAx val="432808664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ellipsometry thickness v Ga intensity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>41.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>106.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>285.37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>547.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>13131</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16549</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19931</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33474</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89404</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171488</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5094-4ADB-8FE8-866C61F1E804}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="573700456"/>
+        <c:axId val="573704392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="573700456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573704392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="573704392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573700456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2138,6 +2610,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4203,6 +4715,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4867,22 +5895,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{387DA0A1-1E89-3E3C-0475-032C360E7AAB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6009473F-92C2-8CF2-5A45-F0CB93016759}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4895,6 +5923,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E6D784C-E49D-8DEF-0BF5-F2794DE7E9AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5202,8 +6266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36829E-C274-49DF-95D4-E8318511F9CD}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5263,6 +6327,9 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
@@ -5298,6 +6365,9 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
@@ -5403,7 +6473,7 @@
         <v>450</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -5450,10 +6520,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2848C461-DB02-413D-AC3C-422114C127E3}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5461,20 +6531,22 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -5491,7 +6563,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>12</v>
@@ -5499,8 +6571,11 @@
       <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3158</v>
       </c>
@@ -5526,7 +6601,7 @@
         <v>340359</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2802</v>
       </c>
@@ -5552,7 +6627,7 @@
         <v>325371</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2808</v>
       </c>
@@ -5578,7 +6653,7 @@
         <v>317822</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2555</v>
       </c>
@@ -5604,7 +6679,7 @@
         <v>291108</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2546</v>
       </c>
@@ -5630,18 +6705,21 @@
         <v>208659</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3076</v>
       </c>
       <c r="C8">
         <v>547.4</v>
+      </c>
+      <c r="D8">
+        <v>171488</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G1:H1"/>
     <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>